<commit_message>
añadidos ejercicios excel 20191105
</commit_message>
<xml_diff>
--- a/m1/unidad3/Practicas/20191029/Basket.xlsx
+++ b/m1/unidad3/Practicas/20191029/Basket.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="145" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Gráfico" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -327,9 +327,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -337,6 +334,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma [0]" xfId="3"/>
@@ -376,35 +376,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>%</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-ES" baseline="0"/>
-              <a:t> Aportación</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -458,7 +430,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-C353-4088-9242-3C6FB6F4EF12}"/>
+                <c16:uniqueId val="{00000001-5103-4A34-8178-F380687BE2E7}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -478,7 +450,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-C353-4088-9242-3C6FB6F4EF12}"/>
+                <c16:uniqueId val="{00000003-5103-4A34-8178-F380687BE2E7}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -498,7 +470,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-C353-4088-9242-3C6FB6F4EF12}"/>
+                <c16:uniqueId val="{00000005-5103-4A34-8178-F380687BE2E7}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -518,7 +490,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-C353-4088-9242-3C6FB6F4EF12}"/>
+                <c16:uniqueId val="{00000007-5103-4A34-8178-F380687BE2E7}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -538,7 +510,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-C353-4088-9242-3C6FB6F4EF12}"/>
+                <c16:uniqueId val="{00000009-5103-4A34-8178-F380687BE2E7}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -558,7 +530,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-C353-4088-9242-3C6FB6F4EF12}"/>
+                <c16:uniqueId val="{0000000B-5103-4A34-8178-F380687BE2E7}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -580,7 +552,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-C353-4088-9242-3C6FB6F4EF12}"/>
+                <c16:uniqueId val="{0000000D-5103-4A34-8178-F380687BE2E7}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -602,7 +574,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000F-C353-4088-9242-3C6FB6F4EF12}"/>
+                <c16:uniqueId val="{0000000F-5103-4A34-8178-F380687BE2E7}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -624,7 +596,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000011-C353-4088-9242-3C6FB6F4EF12}"/>
+                <c16:uniqueId val="{00000011-5103-4A34-8178-F380687BE2E7}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -646,7 +618,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000013-C353-4088-9242-3C6FB6F4EF12}"/>
+                <c16:uniqueId val="{00000013-5103-4A34-8178-F380687BE2E7}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -668,7 +640,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000015-C353-4088-9242-3C6FB6F4EF12}"/>
+                <c16:uniqueId val="{00000015-5103-4A34-8178-F380687BE2E7}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -690,69 +662,10 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000017-C353-4088-9242-3C6FB6F4EF12}"/>
+                <c16:uniqueId val="{00000017-5103-4A34-8178-F380687BE2E7}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dLbls>
-            <c:spPr>
-              <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="25000"/>
-                    <a:lumOff val="75000"/>
-                  </a:sysClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="bestFit"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="1"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <a:prstGeom prst="wedgeRectCallout">
-                    <a:avLst/>
-                  </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                </c15:spPr>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'145'!$D$17:$D$28</c:f>
@@ -844,7 +757,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-313C-4547-89CB-2A552C1FC8AE}"/>
+              <c16:uniqueId val="{00000018-5103-4A34-8178-F380687BE2E7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -855,7 +768,7 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
@@ -867,6 +780,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -876,7 +821,12 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -891,11 +841,6 @@
       <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1458,6 +1403,17 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1881,23 +1837,15 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308171" cy="6078963"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1910,7 +1858,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3041,7 +2989,7 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3063,15 +3011,15 @@
     <row r="1" spans="1:13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="3"/>
       <c r="L1" s="2"/>
       <c r="M1" s="4"/>
@@ -3346,7 +3294,7 @@
         <f t="shared" si="2"/>
         <v>SI</v>
       </c>
-      <c r="S23" s="23"/>
+      <c r="S23" s="22"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B24" s="8"/>
@@ -3569,7 +3517,7 @@
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
       <c r="J37" s="15"/>
-      <c r="K37" s="21">
+      <c r="K37" s="20">
         <f>AVERAGE(I17:I28)</f>
         <v>8.9166666666666661</v>
       </c>
@@ -3622,7 +3570,7 @@
       <c r="J40" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="K40" s="22">
+      <c r="K40" s="21">
         <f>VLOOKUP(J40,D17:I28,2,FALSE)/VLOOKUP(J40,D17:I28,6,FALSE)</f>
         <v>5</v>
       </c>
@@ -3631,7 +3579,7 @@
   <mergeCells count="1">
     <mergeCell ref="C1:I1"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J40">
       <formula1>$D$17:$D$28</formula1>
     </dataValidation>
@@ -3641,19 +3589,4 @@
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>